<commit_message>
Add credit note, re-invoice generation, and qty column support
Adds creditnote.js and creditnote-results.js modules for generating
credit note and corrected re-invoice sheets from exception rows.
Extends column detector with qty aliases and propagates qty/lineTotal
through reconciliation rows. Updates email draft to mention generated
sheets when exceptions exist. Test data updated with Unit Qty column.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/test-data/erp_export.xlsx
+++ b/test-data/erp_export.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="ERP Export" sheetId="1" r:id="rId1"/>
+    <sheet name="Order Lines" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,245 +397,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>SKU</v>
+        <v>Ordered Item</v>
       </c>
       <c r="B1" t="str">
-        <v>Product Name</v>
+        <v>Description</v>
       </c>
       <c r="C1" t="str">
+        <v>Unit Qty</v>
+      </c>
+      <c r="D1" t="str">
         <v>Unit Price</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>TEST001</v>
+        <v>11080V012</v>
       </c>
       <c r="B2" t="str">
-        <v>Widget Alpha</v>
+        <v>Premium 3-Piece Peeler Set</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>12.99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>TEST002</v>
+        <v>11081V003</v>
       </c>
       <c r="B3" t="str">
-        <v>Widget Beta</v>
+        <v>Classic Swivel Peeler</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>9.99</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>TEST003</v>
+        <v>11082V008</v>
       </c>
       <c r="B4" t="str">
-        <v>Widget Gamma</v>
+        <v>Ergonomic Can Opener</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>21.99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>TEST004</v>
+        <v>11083V001</v>
       </c>
       <c r="B5" t="str">
-        <v>Widget Delta</v>
+        <v>Stainless Steel Garlic Press</v>
       </c>
       <c r="C5">
-        <v>8.5</v>
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>15.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>TEST005</v>
+        <v>11084V005</v>
       </c>
       <c r="B6" t="str">
-        <v>Widget Epsilon</v>
+        <v>Locking Tongs 12-Inch</v>
       </c>
       <c r="C6">
-        <v>12.75</v>
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>14.49</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>TEST006</v>
+        <v>11085V002</v>
       </c>
       <c r="B7" t="str">
-        <v>Widget Zeta</v>
+        <v>Silicone Spatula</v>
       </c>
       <c r="C7">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>11.49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>TEST007</v>
+        <v>11086V010</v>
       </c>
       <c r="B8" t="str">
-        <v>Widget Eta</v>
+        <v>Balloon Whisk 11-Inch</v>
       </c>
       <c r="C8">
-        <v>5.99</v>
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>10.99</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>TEST008</v>
+        <v>11087V004</v>
       </c>
       <c r="B9" t="str">
-        <v>Widget Theta</v>
+        <v>3-Piece Mixing Bowl Set</v>
       </c>
       <c r="C9">
-        <v>18.5</v>
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>29.99</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>TEST009</v>
+        <v>11088V006</v>
       </c>
       <c r="B10" t="str">
-        <v>Widget Iota</v>
+        <v>Salad Spinner Large</v>
       </c>
       <c r="C10">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>32.99</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>TEST010</v>
+        <v>11089V001</v>
       </c>
       <c r="B11" t="str">
-        <v>Widget Kappa</v>
+        <v>Measuring Cups Set of 4</v>
       </c>
       <c r="C11">
-        <v>7.25</v>
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>9.49</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>TEST011</v>
+        <v>11090V003</v>
       </c>
       <c r="B12" t="str">
-        <v>Widget Lambda</v>
+        <v>Bamboo Cutting Board</v>
       </c>
       <c r="C12">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>18.99</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>TEST012</v>
+        <v>11091V007</v>
       </c>
       <c r="B13" t="str">
-        <v>Widget Mu</v>
+        <v>Stainless Steel Colander</v>
       </c>
       <c r="C13">
-        <v>9.99</v>
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>16.49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>TEST013</v>
+        <v>11092V002</v>
       </c>
       <c r="B14" t="str">
-        <v>Widget Nu</v>
+        <v>Box Grater 4-Sided</v>
       </c>
       <c r="C14">
-        <v>14.5</v>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>13.99</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>TEST014</v>
+        <v>11093V009</v>
       </c>
       <c r="B15" t="str">
-        <v>Widget Xi</v>
+        <v>Kitchen Shears Heavy Duty</v>
       </c>
       <c r="C15">
-        <v>27.75</v>
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>19.99</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>TEST015</v>
+        <v>11094V001</v>
       </c>
       <c r="B16" t="str">
-        <v>Widget Omicron</v>
+        <v>Flexible Turner</v>
       </c>
       <c r="C16">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>12.49</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>TEST016</v>
+        <v>11095V004</v>
       </c>
       <c r="B17" t="str">
-        <v>Widget Pi</v>
+        <v>Soup Ladle</v>
       </c>
       <c r="C17">
-        <v>6.5</v>
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>11.99</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>TEST017</v>
+        <v>11096V006</v>
       </c>
       <c r="B18" t="str">
-        <v>Widget Rho</v>
+        <v>Potato Masher</v>
       </c>
       <c r="C18">
-        <v>19.99</v>
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <v>13.49</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>TEST018</v>
+        <v>11097V002</v>
       </c>
       <c r="B19" t="str">
-        <v>Widget Sigma</v>
+        <v>Ice Cream Scoop</v>
       </c>
       <c r="C19">
-        <v>31.25</v>
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>10.99</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>TEST019</v>
+        <v>11098V008</v>
       </c>
       <c r="B20" t="str">
-        <v>Widget Tau</v>
+        <v>Pizza Wheel Cutter</v>
       </c>
       <c r="C20">
-        <v>4.75</v>
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>14.99</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>TEST020</v>
+        <v>11099V003</v>
       </c>
       <c r="B21" t="str">
-        <v>Widget Upsilon</v>
+        <v>Bottle Opener</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>7.99</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>